<commit_message>
Fixed watchlist test cases and SteamAbstractBase class with ping test.
</commit_message>
<xml_diff>
--- a/src/test/test-data/WatchlistRATestData.xlsx
+++ b/src/test/test-data/WatchlistRATestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="154">
   <si>
     <t>API</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>OPQA-312||OPQA-312||OPQA-896||OPQA-898||OPQA-897</t>
+  </si>
+  <si>
+    <t>OPQA-1162||OPQA-1163</t>
   </si>
 </sst>
 </file>
@@ -886,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1526,7 +1529,7 @@
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20" s="6" t="s">
-        <v>28</v>
+        <v>153</v>
       </c>
       <c r="J20" s="2" t="s">
         <v>80</v>
@@ -1585,8 +1588,8 @@
       </c>
       <c r="G22"/>
       <c r="H22"/>
-      <c r="I22" s="6" t="s">
-        <v>28</v>
+      <c r="I22" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>85</v>
@@ -1709,8 +1712,8 @@
       </c>
       <c r="G26"/>
       <c r="H26"/>
-      <c r="I26" s="6" t="s">
-        <v>28</v>
+      <c r="I26" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>96</v>

</xml_diff>